<commit_message>
Answers http - https with apache reverse proxy
</commit_message>
<xml_diff>
--- a/3_ManInTheMiddle/Tasks/SPF_DKIM_etc.xlsx
+++ b/3_ManInTheMiddle/Tasks/SPF_DKIM_etc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EducationRappi\Github\CyberSecRappi\3_ManInTheMiddle\Tasks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{83AF63A4-B242-45C4-AED9-D66A9F9ED230}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CB3777C-BE59-459D-AD03-4F3480FBD937}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-48855" yWindow="3225" windowWidth="18315" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="15">
   <si>
     <t>Sender</t>
   </si>
@@ -61,6 +61,15 @@
   </si>
   <si>
     <t xml:space="preserve">yes/no </t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>no</t>
   </si>
 </sst>
 </file>
@@ -389,8 +398,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CA8B12E-33EE-41FE-BE08-0608EFEFDF7F}">
   <dimension ref="C4:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -431,16 +440,16 @@
         <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F5" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="H5" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="3:8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Mail security: analysys SPF, DKIM, DMARC
</commit_message>
<xml_diff>
--- a/3_ManInTheMiddle/Tasks/SPF_DKIM_etc.xlsx
+++ b/3_ManInTheMiddle/Tasks/SPF_DKIM_etc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EducationRappi\Github\CyberSecRappi\3_ManInTheMiddle\Tasks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CB3777C-BE59-459D-AD03-4F3480FBD937}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B4CF06F-CF83-4ED7-AEFA-E58DEFBA58B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-48855" yWindow="3225" windowWidth="18315" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-55635" yWindow="2685" windowWidth="21615" windowHeight="11190" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="18">
   <si>
     <t>Sender</t>
   </si>
@@ -60,9 +60,6 @@
     <t>SSL protection between sender and receiver</t>
   </si>
   <si>
-    <t xml:space="preserve">yes/no </t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
@@ -70,6 +67,18 @@
   </si>
   <si>
     <t>no</t>
+  </si>
+  <si>
+    <t>yes (Hacking lab has DMARC)</t>
+  </si>
+  <si>
+    <t>As long as checks are successful, DMARC entry is not relevant, but it seems to be visible in the mail header (X-Spamd) whether DMARC would have been used.</t>
+  </si>
+  <si>
+    <t>yes (it seems)</t>
+  </si>
+  <si>
+    <t>not clear</t>
   </si>
 </sst>
 </file>
@@ -113,9 +122,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -396,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CA8B12E-33EE-41FE-BE08-0608EFEFDF7F}">
-  <dimension ref="C4:H8"/>
+  <dimension ref="C4:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -440,16 +452,16 @@
         <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" t="s">
         <v>13</v>
-      </c>
-      <c r="H5" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="6" spans="3:8" x14ac:dyDescent="0.3">
@@ -460,16 +472,16 @@
         <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H6" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="3:8" x14ac:dyDescent="0.3">
@@ -480,16 +492,16 @@
         <v>5</v>
       </c>
       <c r="E7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="3:8" x14ac:dyDescent="0.3">
@@ -500,16 +512,22 @@
         <v>6</v>
       </c>
       <c r="E8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G8" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="H8" t="s">
-        <v>11</v>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="3:8" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="F10" s="2"/>
+      <c r="H10" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>